<commit_message>
Update Final Deliverable pubpol 542.xlsx
</commit_message>
<xml_diff>
--- a/Final Deliverable pubpol 542.xlsx
+++ b/Final Deliverable pubpol 542.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niveditaarvind/Desktop/governance_analytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C01E78D-B590-364B-894E-172D1AF5DD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1AEF1C-6780-A04D-9D60-3ED68BC06028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1640" yWindow="500" windowWidth="21600" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>Unit profits</t>
   </si>
@@ -251,6 +251,27 @@
   <si>
     <t>Prof Max: 225 C + 200 FC</t>
   </si>
+  <si>
+    <t xml:space="preserve">25 First Class Seats </t>
+  </si>
+  <si>
+    <t xml:space="preserve">125 Coach Seats </t>
+  </si>
+  <si>
+    <t>C &gt;=40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For C1, C2 and C3 </t>
+  </si>
+  <si>
+    <t>FC + C &lt;=150</t>
+  </si>
+  <si>
+    <t>The Constraints are met</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total seatls 25+125 = 150 </t>
+  </si>
 </sst>
 </file>
 
@@ -309,7 +330,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,6 +373,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -638,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -760,6 +787,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -769,7 +797,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1050,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G25"/>
+  <dimension ref="B2:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1067,15 +1100,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="43" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1191,8 +1224,8 @@
       <c r="B17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
       <c r="E17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1286,6 +1319,34 @@
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="16" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="47" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>